<commit_message>
DemoUI and NONE Kafka Connection
</commit_message>
<xml_diff>
--- a/doc/servicenow/import_incidents_new.xlsx
+++ b/doc/servicenow/import_incidents_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhirt/MY_DOCUMENTS/04_PROJECTS/01_IBM/01_AIOPS/01_CODE/ibm-aiops-deployer_41dev/doc/servicenow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6910E2F9-0480-9A4B-BEAB-0AD53A3652B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F66A69-D5F6-EA4D-A2A7-216D2D68BDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="67720" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -324,7 +324,7 @@
 - Ratings Service is unable to pick up the restart and has to be restarted as well.</t>
   </si>
   <si>
-    <t>CHG0040007</t>
+    <t>CHG0040002</t>
   </si>
 </sst>
 </file>
@@ -704,8 +704,8 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="93" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>